<commit_message>
fixed lifestage for elk/moose bulls - unclassified
</commit_message>
<xml_diff>
--- a/sims/src/observations/caribou/aerial-population-total-count-recruitment-composition-survey/2.1/test-data/Central Selkirks Caribou_Aerial_Population_Total_Count_Recuit_Comp_Survey_1.0.xlsx
+++ b/sims/src/observations/caribou/aerial-population-total-count-recruitment-composition-survey/2.1/test-data/Central Selkirks Caribou_Aerial_Population_Total_Count_Recuit_Comp_Survey_1.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anissa/DevelopmentProjects/biohubbc-utils/sims/src/observations/caribou/aerial-population-total-count-recruitment-composition-survey/2.1/test-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89330664-A8C4-D647-B196-D2857758A1E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{913F7C82-4A1F-8948-A719-FAD82268267B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="-20580" windowWidth="32880" windowHeight="15880" tabRatio="672" activeTab="1" xr2:uid="{EA928297-87AF-4A2F-92BD-649BD8B345BB}"/>
+    <workbookView xWindow="-23040" yWindow="-20960" windowWidth="32880" windowHeight="15880" tabRatio="672" activeTab="2" xr2:uid="{EA928297-87AF-4A2F-92BD-649BD8B345BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Effort &amp; Site Conditions" sheetId="2" r:id="rId1"/>
@@ -2129,7 +2129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="477">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="476">
   <si>
     <t>Date</t>
   </si>
@@ -3554,9 +3554,6 @@
   </si>
   <si>
     <t>def</t>
-  </si>
-  <si>
-    <t>ghi</t>
   </si>
   <si>
     <t>3637</t>
@@ -12063,7 +12060,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CACE0D7-C202-416C-A799-EE712DC4F630}">
   <dimension ref="A1:AV1268"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="X1" sqref="X1"/>
     </sheetView>
   </sheetViews>
@@ -22856,8 +22853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BF3CD49-E68C-4938-B6DF-730C6EE1AE50}">
   <dimension ref="A1:M104"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -22959,7 +22956,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="35" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B3" s="19">
         <v>43540</v>
@@ -22968,7 +22965,7 @@
         <v>210</v>
       </c>
       <c r="D3" s="35" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="E3" s="35" t="s">
         <v>460</v>

</xml_diff>

<commit_message>
updates to moose adult bulls
</commit_message>
<xml_diff>
--- a/sims/src/observations/caribou/aerial-population-total-count-recruitment-composition-survey/2.1/test-data/Central Selkirks Caribou_Aerial_Population_Total_Count_Recuit_Comp_Survey_1.0.xlsx
+++ b/sims/src/observations/caribou/aerial-population-total-count-recruitment-composition-survey/2.1/test-data/Central Selkirks Caribou_Aerial_Population_Total_Count_Recuit_Comp_Survey_1.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anissa/DevelopmentProjects/biohubbc-utils/sims/src/observations/caribou/aerial-population-total-count-recruitment-composition-survey/2.1/test-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{913F7C82-4A1F-8948-A719-FAD82268267B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F38AED-3405-8F4E-BA79-48D67B76D877}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23040" yWindow="-20960" windowWidth="32880" windowHeight="15880" tabRatio="672" activeTab="2" xr2:uid="{EA928297-87AF-4A2F-92BD-649BD8B345BB}"/>
+    <workbookView xWindow="-21400" yWindow="-20960" windowWidth="32880" windowHeight="15880" tabRatio="672" activeTab="1" xr2:uid="{EA928297-87AF-4A2F-92BD-649BD8B345BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Effort &amp; Site Conditions" sheetId="2" r:id="rId1"/>
@@ -662,18 +662,27 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-The longitude of the observation in </t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">The longitude of the observation in </t>
         </r>
         <r>
           <rPr>
             <u/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -682,7 +691,7 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -692,7 +701,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -701,12 +710,31 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>.
-INSTRUCTIONS: No need to enter Lat/Long coordinates if UTM coordinates are provided.</t>
+          <t xml:space="preserve">.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>INSTRUCTIONS: No need to enter Lat/Long coordinates if UTM coordinates are provided.</t>
         </r>
       </text>
     </comment>
@@ -2129,7 +2157,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="476">
   <si>
     <t>Date</t>
   </si>
@@ -3572,7 +3600,7 @@
     <numFmt numFmtId="169" formatCode="hh:mm:ss;@"/>
     <numFmt numFmtId="170" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3660,6 +3688,20 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
@@ -12060,8 +12102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CACE0D7-C202-416C-A799-EE712DC4F630}">
   <dimension ref="A1:AV1268"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X1" sqref="X1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12259,8 +12301,8 @@
       <c r="D2" s="69">
         <v>43540</v>
       </c>
-      <c r="E2" s="60">
-        <v>0.45833333333333331</v>
+      <c r="E2" s="60" t="s">
+        <v>470</v>
       </c>
       <c r="F2" s="16">
         <v>11</v>
@@ -22853,7 +22895,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BF3CD49-E68C-4938-B6DF-730C6EE1AE50}">
   <dimension ref="A1:M104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>

</xml_diff>